<commit_message>
ajuste final nos gráficos do apendice
</commit_message>
<xml_diff>
--- a/table_general_sums.xlsx
+++ b/table_general_sums.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fglopez/Documents/GitHub/a_reguladora/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r1705296\Documents\Git\a_reguladora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD2014D-0ABA-134A-9B35-7A5409D1EA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49306EEB-4D68-43AE-9104-DDEBA207A8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2100" windowWidth="25720" windowHeight="15900" xr2:uid="{FAB62441-014B-5E42-B7BF-77E0BC4133BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FAB62441-014B-5E42-B7BF-77E0BC4133BB}"/>
   </bookViews>
   <sheets>
     <sheet name="tab_general_english" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>year</t>
   </si>
@@ -75,6 +76,48 @@
   </si>
   <si>
     <t>total_servants_officers_otherRAs</t>
+  </si>
+  <si>
+    <t>servants 3 Ras</t>
+  </si>
+  <si>
+    <t>appointees_3RAs</t>
+  </si>
+  <si>
+    <t>toplevel_3RAs</t>
+  </si>
+  <si>
+    <t>servants_otherRAs</t>
+  </si>
+  <si>
+    <t>appointees_otherRAs</t>
+  </si>
+  <si>
+    <t>toplevel_otherRAs</t>
+  </si>
+  <si>
+    <t>servants_officers_3RAs</t>
+  </si>
+  <si>
+    <t>appointees_officers_3RAs</t>
+  </si>
+  <si>
+    <t>toplevel_officers_3RAs</t>
+  </si>
+  <si>
+    <t>servants_officers_otherRAs</t>
+  </si>
+  <si>
+    <t>appointees_officers_otherRAs</t>
+  </si>
+  <si>
+    <t>toplevel_officers_otherRAs</t>
+  </si>
+  <si>
+    <t>total (considering civil and military)</t>
+  </si>
+  <si>
+    <t>total (considering only military)</t>
   </si>
 </sst>
 </file>
@@ -110,13 +153,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,13 +449,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D21F624-AD84-7745-960E-764CC2B32EFB}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +496,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>2013</v>
       </c>
@@ -488,7 +537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2014</v>
       </c>
@@ -529,7 +578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>2015</v>
       </c>
@@ -570,7 +619,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2016</v>
       </c>
@@ -611,7 +660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>2017</v>
       </c>
@@ -652,7 +701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>2018</v>
       </c>
@@ -693,7 +742,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>2019</v>
       </c>
@@ -734,7 +783,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>2020</v>
       </c>
@@ -775,7 +824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>2021</v>
       </c>
@@ -816,7 +865,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>2022</v>
       </c>
@@ -857,7 +906,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>2023</v>
       </c>
@@ -898,7 +947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>2024</v>
       </c>
@@ -942,4 +991,574 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28E600E-4422-4D5A-BFB3-53B9A51CC3FC}">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B3">
+        <v>4029</v>
+      </c>
+      <c r="C3">
+        <v>1106</v>
+      </c>
+      <c r="D3">
+        <v>332</v>
+      </c>
+      <c r="E3">
+        <v>5146</v>
+      </c>
+      <c r="F3">
+        <v>1640</v>
+      </c>
+      <c r="G3">
+        <v>601</v>
+      </c>
+      <c r="H3">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <v>25</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B4">
+        <v>4191</v>
+      </c>
+      <c r="C4">
+        <v>1192</v>
+      </c>
+      <c r="D4">
+        <v>356</v>
+      </c>
+      <c r="E4">
+        <v>5309</v>
+      </c>
+      <c r="F4">
+        <v>1776</v>
+      </c>
+      <c r="G4">
+        <v>650</v>
+      </c>
+      <c r="H4">
+        <v>34</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B5">
+        <v>4406</v>
+      </c>
+      <c r="C5">
+        <v>1222</v>
+      </c>
+      <c r="D5">
+        <v>370</v>
+      </c>
+      <c r="E5">
+        <v>5505</v>
+      </c>
+      <c r="F5">
+        <v>1794</v>
+      </c>
+      <c r="G5">
+        <v>671</v>
+      </c>
+      <c r="H5">
+        <v>42</v>
+      </c>
+      <c r="I5">
+        <v>24</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>22</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B6">
+        <v>4336</v>
+      </c>
+      <c r="C6">
+        <v>1245</v>
+      </c>
+      <c r="D6">
+        <v>380</v>
+      </c>
+      <c r="E6">
+        <v>5633</v>
+      </c>
+      <c r="F6">
+        <v>1903</v>
+      </c>
+      <c r="G6">
+        <v>701</v>
+      </c>
+      <c r="H6">
+        <v>39</v>
+      </c>
+      <c r="I6">
+        <v>23</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <v>29</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B7">
+        <v>4309</v>
+      </c>
+      <c r="C7">
+        <v>1327</v>
+      </c>
+      <c r="D7">
+        <v>398</v>
+      </c>
+      <c r="E7">
+        <v>5545</v>
+      </c>
+      <c r="F7">
+        <v>1932</v>
+      </c>
+      <c r="G7">
+        <v>738</v>
+      </c>
+      <c r="H7">
+        <v>36</v>
+      </c>
+      <c r="I7">
+        <v>22</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>27</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B8">
+        <v>4271</v>
+      </c>
+      <c r="C8">
+        <v>1307</v>
+      </c>
+      <c r="D8">
+        <v>367</v>
+      </c>
+      <c r="E8">
+        <v>5526</v>
+      </c>
+      <c r="F8">
+        <v>1939</v>
+      </c>
+      <c r="G8">
+        <v>747</v>
+      </c>
+      <c r="H8">
+        <v>41</v>
+      </c>
+      <c r="I8">
+        <v>17</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>30</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B9">
+        <v>4129</v>
+      </c>
+      <c r="C9">
+        <v>1327</v>
+      </c>
+      <c r="D9">
+        <v>373</v>
+      </c>
+      <c r="E9">
+        <v>5343</v>
+      </c>
+      <c r="F9">
+        <v>1921</v>
+      </c>
+      <c r="G9">
+        <v>759</v>
+      </c>
+      <c r="H9">
+        <v>35</v>
+      </c>
+      <c r="I9">
+        <v>13</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>27</v>
+      </c>
+      <c r="L9">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B10">
+        <v>3893</v>
+      </c>
+      <c r="C10">
+        <v>1287</v>
+      </c>
+      <c r="D10">
+        <v>377</v>
+      </c>
+      <c r="E10">
+        <v>6197</v>
+      </c>
+      <c r="F10">
+        <v>2158</v>
+      </c>
+      <c r="G10">
+        <v>800</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+      <c r="I10">
+        <v>21</v>
+      </c>
+      <c r="J10">
+        <v>13</v>
+      </c>
+      <c r="K10">
+        <v>26</v>
+      </c>
+      <c r="L10">
+        <v>9</v>
+      </c>
+      <c r="M10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B11">
+        <v>4119</v>
+      </c>
+      <c r="C11">
+        <v>1336</v>
+      </c>
+      <c r="D11">
+        <v>372</v>
+      </c>
+      <c r="E11">
+        <v>6595</v>
+      </c>
+      <c r="F11">
+        <v>2110</v>
+      </c>
+      <c r="G11">
+        <v>812</v>
+      </c>
+      <c r="H11">
+        <v>53</v>
+      </c>
+      <c r="I11">
+        <v>30</v>
+      </c>
+      <c r="J11">
+        <v>20</v>
+      </c>
+      <c r="K11">
+        <v>37</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B12">
+        <v>4120</v>
+      </c>
+      <c r="C12">
+        <v>1320</v>
+      </c>
+      <c r="D12">
+        <v>376</v>
+      </c>
+      <c r="E12">
+        <v>6401</v>
+      </c>
+      <c r="F12">
+        <v>2130</v>
+      </c>
+      <c r="G12">
+        <v>827</v>
+      </c>
+      <c r="H12">
+        <v>51</v>
+      </c>
+      <c r="I12">
+        <v>31</v>
+      </c>
+      <c r="J12">
+        <v>22</v>
+      </c>
+      <c r="K12">
+        <v>28</v>
+      </c>
+      <c r="L12">
+        <v>9</v>
+      </c>
+      <c r="M12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
+        <v>2023</v>
+      </c>
+      <c r="B13">
+        <v>4112</v>
+      </c>
+      <c r="C13">
+        <v>1336</v>
+      </c>
+      <c r="D13">
+        <v>392</v>
+      </c>
+      <c r="E13">
+        <v>6256</v>
+      </c>
+      <c r="F13">
+        <v>2217</v>
+      </c>
+      <c r="G13">
+        <v>892</v>
+      </c>
+      <c r="H13">
+        <v>46</v>
+      </c>
+      <c r="I13">
+        <v>31</v>
+      </c>
+      <c r="J13">
+        <v>22</v>
+      </c>
+      <c r="K13">
+        <v>32</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="2">
+        <v>2024</v>
+      </c>
+      <c r="B14">
+        <v>4084</v>
+      </c>
+      <c r="C14">
+        <v>1343</v>
+      </c>
+      <c r="D14">
+        <v>400</v>
+      </c>
+      <c r="E14">
+        <v>6250</v>
+      </c>
+      <c r="F14">
+        <v>2146</v>
+      </c>
+      <c r="G14">
+        <v>875</v>
+      </c>
+      <c r="H14">
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>16</v>
+      </c>
+      <c r="J14">
+        <v>14</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>